<commit_message>
fix typo and update 308 muzzles sheet
</commit_message>
<xml_diff>
--- a/changes/308-muzzles.xlsx
+++ b/changes/308-muzzles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AAB480-D069-4B31-A1D6-3A6D60FBB485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFC8DE3-ABF2-4756-A960-A456193CEA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="5100" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -721,7 +721,7 @@
   <dimension ref="A1:AI1025"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="3">
         <v>0.7</v>
@@ -955,7 +955,7 @@
       </c>
       <c r="AA3" s="2">
         <f t="shared" ref="AA3:AA66" si="2">P3-Q3*20-R3*0.8-S3*0.6-U3*15+V3*40+W3/300</f>
-        <v>-115.91666666666667</v>
+        <v>-83.916666666666671</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -1307,7 +1307,7 @@
         <v>45</v>
       </c>
       <c r="Q8" s="6">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="R8" s="6">
         <v>70</v>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="AA8" s="2">
         <f t="shared" si="2"/>
-        <v>-45.333333333333336</v>
+        <v>-39.333333333333336</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -2284,10 +2284,10 @@
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="Q20" s="6">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="R20" s="6">
         <v>70</v>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="AA20" s="2">
         <f t="shared" si="2"/>
-        <v>-66.833333333333329</v>
+        <v>-59.833333333333336</v>
       </c>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
@@ -4545,7 +4545,7 @@
         <v>-15</v>
       </c>
       <c r="S48" s="1">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="T48" s="1"/>
       <c r="U48" s="1">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="AA48" s="2">
         <f t="shared" si="2"/>
-        <v>17.733333333333331</v>
+        <v>17.133333333333333</v>
       </c>
       <c r="AB48" s="1"/>
       <c r="AC48" s="3">
@@ -4629,7 +4629,7 @@
         <v>-13</v>
       </c>
       <c r="S49" s="1">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="T49" s="1"/>
       <c r="U49" s="1">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="AA49" s="2">
         <f t="shared" si="2"/>
-        <v>17.466666666666669</v>
+        <v>16.866666666666667</v>
       </c>
       <c r="AB49" s="1"/>
       <c r="AC49" s="3">
@@ -41446,7 +41446,7 @@
       <c r="AI1025" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P3:T66 U3:U63 V3:AA66">
+  <conditionalFormatting sqref="U3:U63 P3:T66 V3:AA66">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>P3&lt;&gt;C3</formula>
     </cfRule>

</xml_diff>

<commit_message>
remove damage penalty from 308 muzzles
</commit_message>
<xml_diff>
--- a/changes/308-muzzles.xlsx
+++ b/changes/308-muzzles.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFC8DE3-ABF2-4756-A960-A456193CEA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AC8FC9B1-F5B4-4BF5-9653-EE82187E6A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="308-muzzles" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
   <si>
     <t>old</t>
   </si>
@@ -439,6 +439,12 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>dsa_warz_series_7.62x51_flash_hider</t>
+  </si>
+  <si>
+    <t>DSA WarZ Series 7.62x51</t>
+  </si>
 </sst>
 </file>
 
@@ -718,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI1025"/>
+  <dimension ref="A1:AI1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -920,7 +926,7 @@
         <v>65000</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" ref="N3:N66" si="1">C3-D3*20-E3*0.8-F3*0.6-H3*15+I3*40+J3/300</f>
+        <f t="shared" ref="N3:N67" si="1">C3-D3*20-E3*0.8-F3*0.6-H3*15+I3*40+J3/300</f>
         <v>-138.06666666666666</v>
       </c>
       <c r="O3" s="1"/>
@@ -931,16 +937,16 @@
         <v>0.7</v>
       </c>
       <c r="R3" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S3" s="3">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
       </c>
       <c r="U3" s="3">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="V3" s="3">
         <v>0.8</v>
@@ -954,8 +960,8 @@
         <v>65000</v>
       </c>
       <c r="AA3" s="2">
-        <f t="shared" ref="AA3:AA66" si="2">P3-Q3*20-R3*0.8-S3*0.6-U3*15+V3*40+W3/300</f>
-        <v>-83.916666666666671</v>
+        <f t="shared" ref="AA3:AA67" si="2">P3-Q3*20-R3*0.8-S3*0.6-U3*15+V3*40+W3/300</f>
+        <v>-69.166666666666671</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -1180,10 +1186,10 @@
         <v>0.06</v>
       </c>
       <c r="R6" s="3">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="S6" s="3">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1">
@@ -1202,7 +1208,7 @@
       </c>
       <c r="AA6" s="2">
         <f t="shared" si="2"/>
-        <v>11.616666666666665</v>
+        <v>14.416666666666666</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
@@ -2160,10 +2166,10 @@
         <v>0.05</v>
       </c>
       <c r="R18" s="3">
+        <v>-11</v>
+      </c>
+      <c r="S18" s="3">
         <v>-9</v>
-      </c>
-      <c r="S18" s="3">
-        <v>-7</v>
       </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1">
@@ -2182,7 +2188,7 @@
       </c>
       <c r="AA18" s="2">
         <f t="shared" si="2"/>
-        <v>11.566666666666666</v>
+        <v>14.366666666666665</v>
       </c>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
@@ -2284,7 +2290,7 @@
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="6">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="6">
         <v>0.7</v>
@@ -2293,13 +2299,13 @@
         <v>70</v>
       </c>
       <c r="S20" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="T20" s="6">
         <v>0</v>
       </c>
       <c r="U20" s="6">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="V20" s="6">
         <v>0.8</v>
@@ -2314,7 +2320,7 @@
       </c>
       <c r="AA20" s="2">
         <f t="shared" si="2"/>
-        <v>-59.833333333333336</v>
+        <v>-57.333333333333336</v>
       </c>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
@@ -3668,13 +3674,13 @@
         <v>1</v>
       </c>
       <c r="Q37" s="3">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="R37" s="3">
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="S37" s="3">
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="3">
@@ -3693,7 +3699,7 @@
       </c>
       <c r="AA37" s="2">
         <f t="shared" si="2"/>
-        <v>12.1</v>
+        <v>15.499999999999998</v>
       </c>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
@@ -3709,114 +3715,107 @@
     </row>
     <row r="38" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="C38" s="1">
-        <v>-2.5</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="E38" s="1">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="F38" s="1">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="G38" s="1"/>
-      <c r="H38" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="1">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="N38" s="2">
         <f t="shared" si="1"/>
-        <v>2.4833333333333334</v>
+        <v>9.8833333333333346</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q38" s="3">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="R38" s="3">
         <v>-9</v>
       </c>
       <c r="S38" s="3">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="T38" s="1"/>
-      <c r="U38" s="3">
+      <c r="U38" s="6">
         <v>0</v>
       </c>
-      <c r="V38" s="1">
+      <c r="V38" s="6">
         <v>0</v>
       </c>
       <c r="W38" s="1">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="1">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="AA38" s="2">
         <f t="shared" si="2"/>
-        <v>12.833333333333334</v>
+        <v>15.283333333333333</v>
       </c>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
+      <c r="AF38" s="3"/>
       <c r="AG38" s="1"/>
       <c r="AH38" s="1"/>
-      <c r="AI38" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="AI38" s="3"/>
     </row>
     <row r="39" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39" s="1">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="D39" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E39" s="1">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="F39" s="1">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="I39" s="1">
         <v>0</v>
       </c>
       <c r="J39" s="1">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -3825,30 +3824,30 @@
       </c>
       <c r="N39" s="2">
         <f t="shared" si="1"/>
-        <v>2.5666666666666664</v>
+        <v>2.4833333333333334</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q39" s="3">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="R39" s="3">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="S39" s="3">
-        <v>-7</v>
+        <v>-14</v>
       </c>
       <c r="T39" s="1"/>
-      <c r="U39" s="1">
+      <c r="U39" s="3">
         <v>0</v>
       </c>
       <c r="V39" s="1">
         <v>0</v>
       </c>
       <c r="W39" s="1">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
@@ -3857,7 +3856,7 @@
       </c>
       <c r="AA39" s="2">
         <f t="shared" si="2"/>
-        <v>11.966666666666667</v>
+        <v>16.033333333333335</v>
       </c>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
@@ -3873,73 +3872,73 @@
     </row>
     <row r="40" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" s="1">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D40" s="1">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E40" s="1">
-        <v>17</v>
+        <v>-2</v>
       </c>
       <c r="F40" s="1">
-        <v>-34</v>
+        <v>-7</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="N40" s="2">
         <f t="shared" si="1"/>
-        <v>-6.5000000000000036</v>
+        <v>2.5666666666666664</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="3">
-        <v>-3</v>
-      </c>
-      <c r="Q40" s="1">
-        <v>0.04</v>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>0.06</v>
       </c>
       <c r="R40" s="3">
-        <v>10</v>
+        <v>-13</v>
       </c>
       <c r="S40" s="3">
-        <v>-20</v>
+        <v>-11</v>
       </c>
       <c r="T40" s="1"/>
-      <c r="U40" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V40" s="3">
-        <v>-0.02</v>
+      <c r="U40" s="1">
+        <v>0</v>
+      </c>
+      <c r="V40" s="1">
+        <v>0</v>
       </c>
       <c r="W40" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="AA40" s="2">
         <f t="shared" si="2"/>
-        <v>-3.6000000000000005</v>
+        <v>15.966666666666667</v>
       </c>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
@@ -3999,10 +3998,10 @@
         <v>0.06</v>
       </c>
       <c r="R41" s="3">
-        <v>-8</v>
+        <v>-11</v>
       </c>
       <c r="S41" s="3">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="T41" s="1"/>
       <c r="U41" s="1">
@@ -4021,7 +4020,7 @@
       </c>
       <c r="AA41" s="2">
         <f t="shared" si="2"/>
-        <v>12.966666666666667</v>
+        <v>15.966666666666667</v>
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
@@ -4078,10 +4077,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="R42" s="3">
+        <v>-14</v>
+      </c>
+      <c r="S42" s="3">
         <v>-10</v>
-      </c>
-      <c r="S42" s="3">
-        <v>-9</v>
       </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1">
@@ -4100,14 +4099,14 @@
       </c>
       <c r="AA42" s="2">
         <f t="shared" si="2"/>
-        <v>13.166666666666666</v>
+        <v>16.966666666666669</v>
       </c>
       <c r="AB42" s="1"/>
       <c r="AC42" s="3">
         <v>4.25</v>
       </c>
       <c r="AD42" s="1">
-        <f t="shared" ref="AD42:AD59" si="5">AC42*0.015</f>
+        <f t="shared" ref="AD42:AD60" si="5">AC42*0.015</f>
         <v>6.3750000000000001E-2</v>
       </c>
       <c r="AE42" s="1"/>
@@ -4162,17 +4161,17 @@
         <v>0.06</v>
       </c>
       <c r="R43" s="3">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="S43" s="3">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="T43" s="1"/>
       <c r="U43" s="3">
         <v>0.05</v>
       </c>
       <c r="V43" s="3">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="W43" s="1">
         <v>20</v>
@@ -4184,7 +4183,7 @@
       </c>
       <c r="AA43" s="2">
         <f t="shared" si="2"/>
-        <v>14.916666666666666</v>
+        <v>16.716666666666665</v>
       </c>
       <c r="AB43" s="1"/>
       <c r="AC43" s="3">
@@ -4240,23 +4239,23 @@
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="Q44" s="3">
         <v>0.06</v>
       </c>
       <c r="R44" s="3">
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="S44" s="3">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="T44" s="1"/>
       <c r="U44" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="V44" s="3">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
       <c r="W44" s="1">
         <v>30</v>
@@ -4268,7 +4267,7 @@
       </c>
       <c r="AA44" s="2">
         <f t="shared" si="2"/>
-        <v>15.050000000000002</v>
+        <v>16.950000000000003</v>
       </c>
       <c r="AB44" s="1"/>
       <c r="AC44" s="3">
@@ -4330,17 +4329,17 @@
         <v>0.05</v>
       </c>
       <c r="R45" s="3">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="S45" s="3">
         <v>-15</v>
       </c>
       <c r="T45" s="1"/>
       <c r="U45" s="3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="V45" s="3">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
       <c r="W45" s="1">
         <v>30</v>
@@ -4352,7 +4351,7 @@
       </c>
       <c r="AA45" s="2">
         <f t="shared" si="2"/>
-        <v>14.4</v>
+        <v>16.75</v>
       </c>
       <c r="AB45" s="1"/>
       <c r="AC45" s="3">
@@ -4370,19 +4369,19 @@
     </row>
     <row r="46" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C46" s="1">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="D46" s="1">
-        <v>0.17</v>
+        <v>0.04</v>
       </c>
       <c r="E46" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F46" s="1">
         <v>-34</v>
@@ -4392,97 +4391,133 @@
         <v>0.3</v>
       </c>
       <c r="I46" s="1">
-        <v>-0.02</v>
+        <v>-0.1</v>
       </c>
       <c r="J46" s="1">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="N46" s="2">
-        <f t="shared" si="1"/>
-        <v>-4.7666666666666684</v>
+        <f>C46-D46*20-E46*0.8-F46*0.6-H46*15+I46*40+J46/300</f>
+        <v>-6.5000000000000036</v>
       </c>
       <c r="O46" s="1"/>
-      <c r="P46" s="1">
-        <v>-6</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>0.16</v>
+      <c r="P46" s="3">
+        <v>-3</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>0.04</v>
       </c>
       <c r="R46" s="3">
-        <v>12</v>
-      </c>
-      <c r="S46" s="1">
-        <v>-34</v>
+        <v>14</v>
+      </c>
+      <c r="S46" s="3">
+        <v>-22</v>
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="3">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="V46" s="3">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="W46" s="1">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
       <c r="Z46" s="1">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="AA46" s="2">
-        <f t="shared" si="2"/>
-        <v>-1.9166666666666687</v>
+        <f>P46-Q46*20-R46*0.8-S46*0.6-U46*15+V46*40+W46/300</f>
+        <v>-3.7000000000000006</v>
       </c>
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
-      <c r="AD46" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="AD46" s="1"/>
       <c r="AE46" s="1"/>
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
-      <c r="AI46" s="1"/>
+      <c r="AI46" s="3">
+        <f>AF46+AG46*0.038+AH46</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="1">
+        <v>-6</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="E47" s="1">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1">
+        <v>-34</v>
+      </c>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
+      <c r="H47" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I47" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="J47" s="1">
+        <v>-20</v>
+      </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
+      <c r="M47" s="1">
+        <v>1500</v>
+      </c>
       <c r="N47" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-4.7666666666666684</v>
       </c>
       <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
+      <c r="P47" s="1">
+        <v>-6</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="R47" s="3">
+        <v>10</v>
+      </c>
+      <c r="S47" s="1">
+        <v>-35</v>
+      </c>
       <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
+      <c r="U47" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="V47" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="W47" s="1">
+        <v>-20</v>
+      </c>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
+      <c r="Z47" s="1">
+        <v>1500</v>
+      </c>
       <c r="AA47" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.0833333333333341</v>
       </c>
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
@@ -4497,82 +4532,44 @@
       <c r="AI47" s="1"/>
     </row>
     <row r="48" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="1">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E48" s="1">
-        <v>-15</v>
-      </c>
-      <c r="F48" s="1">
-        <v>-12</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1">
-        <v>0</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="J48" s="1">
-        <v>40</v>
-      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="1">
-        <v>1000</v>
-      </c>
+      <c r="M48" s="1"/>
       <c r="N48" s="2">
         <f t="shared" si="1"/>
-        <v>17.733333333333331</v>
+        <v>0</v>
       </c>
       <c r="O48" s="1"/>
-      <c r="P48" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="R48" s="1">
-        <v>-15</v>
-      </c>
-      <c r="S48" s="1">
-        <v>-11</v>
-      </c>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
       <c r="T48" s="1"/>
-      <c r="U48" s="1">
-        <v>0</v>
-      </c>
-      <c r="V48" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="W48" s="1">
-        <v>40</v>
-      </c>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
-      <c r="Z48" s="1">
-        <v>1000</v>
-      </c>
+      <c r="Z48" s="1"/>
       <c r="AA48" s="2">
         <f t="shared" si="2"/>
-        <v>17.133333333333333</v>
+        <v>0</v>
       </c>
       <c r="AB48" s="1"/>
-      <c r="AC48" s="3">
-        <v>7.8</v>
-      </c>
+      <c r="AC48" s="1"/>
       <c r="AD48" s="1">
         <f t="shared" si="5"/>
-        <v>0.11699999999999999</v>
+        <v>0</v>
       </c>
       <c r="AE48" s="1"/>
       <c r="AF48" s="1"/>
@@ -4582,22 +4579,22 @@
     </row>
     <row r="49" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="1">
         <v>0</v>
       </c>
       <c r="D49" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="E49" s="1">
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="F49" s="1">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1">
@@ -4607,7 +4604,7 @@
         <v>0.02</v>
       </c>
       <c r="J49" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -4616,20 +4613,20 @@
       </c>
       <c r="N49" s="2">
         <f t="shared" si="1"/>
-        <v>17.466666666666669</v>
+        <v>17.733333333333331</v>
       </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1">
         <v>0</v>
       </c>
       <c r="Q49" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="R49" s="1">
+        <v>-17</v>
+      </c>
+      <c r="S49" s="1">
         <v>-13</v>
-      </c>
-      <c r="S49" s="1">
-        <v>-14</v>
       </c>
       <c r="T49" s="1"/>
       <c r="U49" s="1">
@@ -4639,7 +4636,7 @@
         <v>0.02</v>
       </c>
       <c r="W49" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
@@ -4648,15 +4645,15 @@
       </c>
       <c r="AA49" s="2">
         <f t="shared" si="2"/>
-        <v>16.866666666666667</v>
+        <v>19.933333333333334</v>
       </c>
       <c r="AB49" s="1"/>
       <c r="AC49" s="3">
-        <v>9.5</v>
+        <v>7.8</v>
       </c>
       <c r="AD49" s="1">
         <f t="shared" si="5"/>
-        <v>0.14249999999999999</v>
+        <v>0.11699999999999999</v>
       </c>
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>
@@ -4664,45 +4661,83 @@
       <c r="AH49" s="1"/>
       <c r="AI49" s="1"/>
     </row>
-    <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+    <row r="50" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E50" s="1">
+        <v>-13</v>
+      </c>
+      <c r="F50" s="1">
+        <v>-15</v>
+      </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="J50" s="1">
+        <v>20</v>
+      </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
+      <c r="M50" s="1">
+        <v>1000</v>
+      </c>
       <c r="N50" s="2">
         <f t="shared" si="1"/>
+        <v>17.466666666666669</v>
+      </c>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1">
         <v>0</v>
       </c>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
+      <c r="Q50" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R50" s="1">
+        <v>-15</v>
+      </c>
+      <c r="S50" s="1">
+        <v>-16</v>
+      </c>
       <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
+      <c r="U50" s="1">
+        <v>0</v>
+      </c>
+      <c r="V50" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="W50" s="1">
+        <v>20</v>
+      </c>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
+      <c r="Z50" s="1">
+        <v>1000</v>
+      </c>
       <c r="AA50" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>19.666666666666664</v>
       </c>
       <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
+      <c r="AC50" s="3">
+        <v>9.5</v>
+      </c>
       <c r="AD50" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="AE50" s="1"/>
       <c r="AF50" s="1"/>
@@ -4710,83 +4745,45 @@
       <c r="AH50" s="1"/>
       <c r="AI50" s="1"/>
     </row>
-    <row r="51" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="4">
-        <v>-6</v>
-      </c>
-      <c r="D51" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="E51" s="4">
-        <v>-6</v>
-      </c>
-      <c r="F51" s="4">
-        <v>-10</v>
-      </c>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4">
-        <v>-0.3</v>
-      </c>
-      <c r="I51" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="J51" s="4">
-        <v>200</v>
-      </c>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4">
-        <v>2000</v>
-      </c>
+    <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
       <c r="N51" s="2">
         <f t="shared" si="1"/>
-        <v>8.1666666666666679</v>
+        <v>0</v>
       </c>
       <c r="O51" s="1"/>
-      <c r="P51" s="4">
-        <v>-6</v>
-      </c>
-      <c r="Q51" s="4">
-        <v>0.26</v>
-      </c>
-      <c r="R51" s="8">
-        <v>-8</v>
-      </c>
-      <c r="S51" s="8">
-        <v>-10</v>
-      </c>
-      <c r="T51" s="4"/>
-      <c r="U51" s="8">
-        <v>-0.12</v>
-      </c>
-      <c r="V51" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="W51" s="4">
-        <v>200</v>
-      </c>
-      <c r="X51" s="4"/>
-      <c r="Y51" s="4"/>
-      <c r="Z51" s="4">
-        <v>2000</v>
-      </c>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
       <c r="AA51" s="2">
         <f t="shared" si="2"/>
-        <v>5.6666666666666679</v>
+        <v>0</v>
       </c>
       <c r="AB51" s="1"/>
-      <c r="AC51" s="1">
-        <v>17.600000000000001</v>
-      </c>
+      <c r="AC51" s="1"/>
       <c r="AD51" s="1">
         <f t="shared" si="5"/>
-        <v>0.26400000000000001</v>
+        <v>0</v>
       </c>
       <c r="AE51" s="1"/>
       <c r="AF51" s="1"/>
@@ -4796,81 +4793,81 @@
     </row>
     <row r="52" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C52" s="4">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="D52" s="4">
-        <v>0.21</v>
+        <v>0.25</v>
       </c>
       <c r="E52" s="4">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="F52" s="4">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="I52" s="4">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="J52" s="4">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="N52" s="2">
         <f t="shared" si="1"/>
-        <v>3.1000000000000005</v>
+        <v>8.1666666666666679</v>
       </c>
       <c r="O52" s="1"/>
       <c r="P52" s="4">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="Q52" s="4">
-        <v>0.16</v>
+        <v>0.26</v>
       </c>
       <c r="R52" s="8">
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="S52" s="8">
-        <v>-7</v>
+        <v>-12</v>
       </c>
       <c r="T52" s="4"/>
-      <c r="U52" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="V52" s="4">
-        <v>0.03</v>
+      <c r="U52" s="8">
+        <v>-0.12</v>
+      </c>
+      <c r="V52" s="8">
+        <v>0.05</v>
       </c>
       <c r="W52" s="4">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="X52" s="4"/>
       <c r="Y52" s="4"/>
       <c r="Z52" s="4">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="AA52" s="2">
         <f t="shared" si="2"/>
-        <v>5.8000000000000007</v>
+        <v>8.4666666666666668</v>
       </c>
       <c r="AB52" s="1"/>
       <c r="AC52" s="1">
-        <v>11.3</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="AD52" s="1">
         <f t="shared" si="5"/>
-        <v>0.16950000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="AE52" s="1"/>
       <c r="AF52" s="1"/>
@@ -4880,16 +4877,16 @@
     </row>
     <row r="53" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C53" s="4">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="D53" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="E53" s="4">
         <v>-4</v>
@@ -4910,49 +4907,51 @@
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="N53" s="2">
         <f t="shared" si="1"/>
-        <v>5.4999999999999991</v>
+        <v>3.1000000000000005</v>
       </c>
       <c r="O53" s="1"/>
       <c r="P53" s="4">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="Q53" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="R53" s="8">
-        <v>-2</v>
-      </c>
-      <c r="S53" s="4">
-        <v>-2</v>
+        <v>-9</v>
+      </c>
+      <c r="S53" s="8">
+        <v>-9</v>
       </c>
       <c r="T53" s="4"/>
       <c r="U53" s="4">
-        <v>-0.08</v>
+        <v>-0.1</v>
       </c>
       <c r="V53" s="4">
         <v>0.03</v>
       </c>
       <c r="W53" s="4">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="X53" s="4"/>
       <c r="Y53" s="4"/>
       <c r="Z53" s="4">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="AA53" s="2">
         <f t="shared" si="2"/>
-        <v>-0.16666666666666763</v>
+        <v>8.6</v>
       </c>
       <c r="AB53" s="1"/>
-      <c r="AC53" s="1"/>
+      <c r="AC53" s="1">
+        <v>11.3</v>
+      </c>
       <c r="AD53" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.16950000000000001</v>
       </c>
       <c r="AE53" s="1"/>
       <c r="AF53" s="1"/>
@@ -4962,81 +4961,79 @@
     </row>
     <row r="54" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C54" s="4">
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="D54" s="4">
-        <v>0.28999999999999998</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E54" s="4">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="F54" s="4">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="I54" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J54" s="4">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="N54" s="2">
         <f t="shared" si="1"/>
-        <v>-0.76666666666666727</v>
+        <v>5.4999999999999991</v>
       </c>
       <c r="O54" s="1"/>
       <c r="P54" s="4">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="Q54" s="4">
-        <v>0.21</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R54" s="8">
-        <v>-6</v>
-      </c>
-      <c r="S54" s="8">
-        <v>-11</v>
+        <v>-4</v>
+      </c>
+      <c r="S54" s="4">
+        <v>-4</v>
       </c>
       <c r="T54" s="4"/>
-      <c r="U54" s="8">
-        <v>-0.1</v>
+      <c r="U54" s="4">
+        <v>-0.08</v>
       </c>
       <c r="V54" s="4">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="W54" s="4">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="X54" s="4"/>
       <c r="Y54" s="4"/>
       <c r="Z54" s="4">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="AA54" s="2">
         <f t="shared" si="2"/>
-        <v>6.0333333333333341</v>
+        <v>2.6333333333333329</v>
       </c>
       <c r="AB54" s="1"/>
-      <c r="AC54" s="1">
-        <v>9.1999999999999993</v>
-      </c>
+      <c r="AC54" s="1"/>
       <c r="AD54" s="1">
         <f t="shared" si="5"/>
-        <v>0.13799999999999998</v>
+        <v>0</v>
       </c>
       <c r="AE54" s="1"/>
       <c r="AF54" s="1"/>
@@ -5046,10 +5043,10 @@
     </row>
     <row r="55" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="4">
         <v>-8</v>
@@ -5090,10 +5087,10 @@
         <v>0.21</v>
       </c>
       <c r="R55" s="8">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="S55" s="8">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="T55" s="4"/>
       <c r="U55" s="8">
@@ -5112,13 +5109,15 @@
       </c>
       <c r="AA55" s="2">
         <f t="shared" si="2"/>
-        <v>6.0333333333333341</v>
+        <v>8.8333333333333339</v>
       </c>
       <c r="AB55" s="1"/>
-      <c r="AC55" s="1"/>
+      <c r="AC55" s="1">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="AD55" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.13799999999999998</v>
       </c>
       <c r="AE55" s="1"/>
       <c r="AF55" s="1"/>
@@ -5127,82 +5126,80 @@
       <c r="AI55" s="1"/>
     </row>
     <row r="56" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="1">
-        <v>-2</v>
-      </c>
-      <c r="D56" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="E56" s="1">
-        <v>-2</v>
-      </c>
-      <c r="F56" s="1">
-        <v>-4</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1">
-        <v>-0.05</v>
-      </c>
-      <c r="I56" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="J56" s="1">
-        <v>20</v>
-      </c>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1">
+      <c r="A56" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="4">
+        <v>-8</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E56" s="4">
+        <v>-3</v>
+      </c>
+      <c r="F56" s="4">
+        <v>-8</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="I56" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J56" s="4">
+        <v>100</v>
+      </c>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4">
         <v>1500</v>
       </c>
       <c r="N56" s="2">
         <f t="shared" si="1"/>
-        <v>1.6166666666666665</v>
+        <v>-0.76666666666666727</v>
       </c>
       <c r="O56" s="1"/>
-      <c r="P56" s="1">
-        <v>-3</v>
-      </c>
-      <c r="Q56" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="R56" s="3">
-        <v>-7</v>
-      </c>
-      <c r="S56" s="3">
+      <c r="P56" s="4">
         <v>-5</v>
       </c>
-      <c r="T56" s="1"/>
-      <c r="U56" s="3">
-        <v>-0.06</v>
-      </c>
-      <c r="V56" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="W56" s="1">
-        <v>120</v>
-      </c>
-      <c r="X56" s="1"/>
-      <c r="Y56" s="1"/>
-      <c r="Z56" s="1">
+      <c r="Q56" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="R56" s="8">
+        <v>-8</v>
+      </c>
+      <c r="S56" s="8">
+        <v>-13</v>
+      </c>
+      <c r="T56" s="4"/>
+      <c r="U56" s="8">
+        <v>-0.1</v>
+      </c>
+      <c r="V56" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="W56" s="4">
+        <v>100</v>
+      </c>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4">
         <v>1500</v>
       </c>
       <c r="AA56" s="2">
         <f t="shared" si="2"/>
-        <v>6.1</v>
+        <v>8.8333333333333339</v>
       </c>
       <c r="AB56" s="1"/>
-      <c r="AC56" s="1">
-        <v>7</v>
-      </c>
+      <c r="AC56" s="1"/>
       <c r="AD56" s="1">
         <f t="shared" si="5"/>
-        <v>0.105</v>
+        <v>0</v>
       </c>
       <c r="AE56" s="1"/>
       <c r="AF56" s="1"/>
@@ -5212,79 +5209,81 @@
     </row>
     <row r="57" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C57" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E57" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F57" s="1">
         <v>-4</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E57" s="1">
-        <v>-5</v>
-      </c>
-      <c r="F57" s="1">
-        <v>-5</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="I57" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J57" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="N57" s="2">
         <f t="shared" si="1"/>
-        <v>4.666666666666667</v>
+        <v>1.6166666666666665</v>
       </c>
       <c r="O57" s="1"/>
       <c r="P57" s="1">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="Q57" s="1">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="R57" s="3">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="S57" s="3">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="T57" s="1"/>
       <c r="U57" s="3">
-        <v>-0.11</v>
+        <v>-0.06</v>
       </c>
       <c r="V57" s="3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="W57" s="1">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
       <c r="Z57" s="1">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="AA57" s="2">
         <f t="shared" si="2"/>
-        <v>6.1833333333333336</v>
+        <v>8.9</v>
       </c>
       <c r="AB57" s="1"/>
-      <c r="AC57" s="1"/>
+      <c r="AC57" s="1">
+        <v>7</v>
+      </c>
       <c r="AD57" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.105</v>
       </c>
       <c r="AE57" s="1"/>
       <c r="AF57" s="1"/>
@@ -5294,81 +5293,79 @@
     </row>
     <row r="58" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C58" s="1">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="D58" s="1">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="E58" s="1">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="F58" s="1">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1">
-        <v>-0.15</v>
+        <v>-0.1</v>
       </c>
       <c r="I58" s="1">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="J58" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="N58" s="2">
         <f t="shared" si="1"/>
-        <v>6.9166666666666661</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="O58" s="1"/>
       <c r="P58" s="1">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="Q58" s="1">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="R58" s="3">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="S58" s="3">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="T58" s="1"/>
       <c r="U58" s="3">
-        <v>-0.16</v>
-      </c>
-      <c r="V58" s="1">
-        <v>0.06</v>
+        <v>-0.11</v>
+      </c>
+      <c r="V58" s="3">
+        <v>0.05</v>
       </c>
       <c r="W58" s="1">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
       <c r="Z58" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="AA58" s="2">
         <f t="shared" si="2"/>
-        <v>6.2666666666666675</v>
+        <v>8.9833333333333325</v>
       </c>
       <c r="AB58" s="1"/>
-      <c r="AC58" s="1">
-        <v>11</v>
-      </c>
+      <c r="AC58" s="1"/>
       <c r="AD58" s="1">
         <f t="shared" si="5"/>
-        <v>0.16499999999999998</v>
+        <v>0</v>
       </c>
       <c r="AE58" s="1"/>
       <c r="AF58" s="1"/>
@@ -5377,82 +5374,82 @@
       <c r="AI58" s="1"/>
     </row>
     <row r="59" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" s="4">
-        <v>-3</v>
-      </c>
-      <c r="D59" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="E59" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F59" s="4">
-        <v>8</v>
-      </c>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="I59" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="J59" s="4">
-        <v>-30</v>
-      </c>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4">
-        <v>700</v>
+      <c r="A59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="1">
+        <v>-6</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E59" s="1">
+        <v>-7</v>
+      </c>
+      <c r="F59" s="1">
+        <v>-8</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1">
+        <v>-0.15</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="J59" s="1">
+        <v>80</v>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1">
+        <v>3000</v>
       </c>
       <c r="N59" s="2">
         <f t="shared" si="1"/>
-        <v>-7.7499999999999991</v>
+        <v>6.9166666666666661</v>
       </c>
       <c r="O59" s="1"/>
-      <c r="P59" s="8">
-        <v>-1</v>
-      </c>
-      <c r="Q59" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="R59" s="8">
-        <v>-2</v>
-      </c>
-      <c r="S59" s="8">
-        <v>-5</v>
-      </c>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="V59" s="8">
-        <v>-0.03</v>
-      </c>
-      <c r="W59" s="4">
-        <v>-30</v>
-      </c>
-      <c r="X59" s="4"/>
-      <c r="Y59" s="4"/>
-      <c r="Z59" s="4">
-        <v>700</v>
+      <c r="P59" s="1">
+        <v>-7</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="R59" s="3">
+        <v>-11</v>
+      </c>
+      <c r="S59" s="3">
+        <v>-9</v>
+      </c>
+      <c r="T59" s="1"/>
+      <c r="U59" s="3">
+        <v>-0.16</v>
+      </c>
+      <c r="V59" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="W59" s="1">
+        <v>200</v>
+      </c>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1">
+        <v>3000</v>
       </c>
       <c r="AA59" s="2">
         <f t="shared" si="2"/>
-        <v>0.55000000000000016</v>
+        <v>9.0666666666666664</v>
       </c>
       <c r="AB59" s="1"/>
       <c r="AC59" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="AD59" s="1">
         <f t="shared" si="5"/>
-        <v>0.03</v>
+        <v>0.16499999999999998</v>
       </c>
       <c r="AE59" s="1"/>
       <c r="AF59" s="1"/>
@@ -5462,10 +5459,10 @@
     </row>
     <row r="60" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C60" s="4">
         <v>-3</v>
@@ -5474,17 +5471,17 @@
         <v>0.08</v>
       </c>
       <c r="E60" s="4">
-        <v>-22</v>
+        <v>-10</v>
       </c>
       <c r="F60" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4">
         <v>0.15</v>
       </c>
       <c r="I60" s="4">
-        <v>-0.15</v>
+        <v>-0.1</v>
       </c>
       <c r="J60" s="4">
         <v>-30</v>
@@ -5492,31 +5489,31 @@
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="N60" s="2">
         <f t="shared" si="1"/>
-        <v>-4.9499999999999975</v>
+        <v>-7.7499999999999991</v>
       </c>
       <c r="O60" s="1"/>
-      <c r="P60" s="4">
+      <c r="P60" s="8">
         <v>-1</v>
       </c>
       <c r="Q60" s="4">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="R60" s="8">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="S60" s="8">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="T60" s="4"/>
-      <c r="U60" s="8">
-        <v>0</v>
-      </c>
-      <c r="V60" s="4">
-        <v>0</v>
+      <c r="U60" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="V60" s="8">
+        <v>-0.03</v>
       </c>
       <c r="W60" s="4">
         <v>-30</v>
@@ -5524,15 +5521,20 @@
       <c r="X60" s="4"/>
       <c r="Y60" s="4"/>
       <c r="Z60" s="4">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="AA60" s="2">
         <f t="shared" si="2"/>
-        <v>6.5000000000000009</v>
+        <v>3.35</v>
       </c>
       <c r="AB60" s="1"/>
-      <c r="AC60" s="1"/>
-      <c r="AD60" s="1"/>
+      <c r="AC60" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD60" s="1">
+        <f t="shared" si="5"/>
+        <v>0.03</v>
+      </c>
       <c r="AE60" s="1"/>
       <c r="AF60" s="1"/>
       <c r="AG60" s="1"/>
@@ -5541,82 +5543,77 @@
     </row>
     <row r="61" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C61" s="4">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="D61" s="4">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="E61" s="4">
-        <v>-6</v>
+        <v>-22</v>
       </c>
       <c r="F61" s="4">
-        <v>-10</v>
+        <v>16</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4">
-        <v>-0.3</v>
+        <v>0.15</v>
       </c>
       <c r="I61" s="4">
-        <v>0.08</v>
+        <v>-0.15</v>
       </c>
       <c r="J61" s="4">
-        <v>200</v>
+        <v>-30</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="N61" s="2">
         <f t="shared" si="1"/>
-        <v>8.5666666666666664</v>
+        <v>-4.9499999999999975</v>
       </c>
       <c r="O61" s="1"/>
       <c r="P61" s="4">
-        <v>-6</v>
-      </c>
-      <c r="Q61" s="8">
-        <v>0.2</v>
+        <v>-1</v>
+      </c>
+      <c r="Q61" s="4">
+        <v>0.04</v>
       </c>
       <c r="R61" s="8">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="S61" s="8">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="T61" s="4"/>
-      <c r="U61" s="4">
-        <v>-0.15</v>
-      </c>
-      <c r="V61" s="8">
-        <v>0.04</v>
+      <c r="U61" s="8">
+        <v>0</v>
+      </c>
+      <c r="V61" s="4">
+        <v>0</v>
       </c>
       <c r="W61" s="4">
-        <v>140</v>
+        <v>-30</v>
       </c>
       <c r="X61" s="4"/>
       <c r="Y61" s="4"/>
       <c r="Z61" s="4">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="AA61" s="2">
         <f t="shared" si="2"/>
-        <v>7.7166666666666668</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AB61" s="1"/>
-      <c r="AC61" s="3">
-        <v>13.7</v>
-      </c>
-      <c r="AD61" s="1">
-        <f>AC61*0.015</f>
-        <v>0.20549999999999999</v>
-      </c>
+      <c r="AC61" s="1"/>
+      <c r="AD61" s="1"/>
       <c r="AE61" s="1"/>
       <c r="AF61" s="1"/>
       <c r="AG61" s="1"/>
@@ -5625,57 +5622,82 @@
     </row>
     <row r="62" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C62" s="4">
-        <v>-0.5</v>
+        <v>-6</v>
       </c>
       <c r="D62" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+        <v>0.23</v>
+      </c>
+      <c r="E62" s="4">
+        <v>-6</v>
+      </c>
+      <c r="F62" s="4">
+        <v>-10</v>
+      </c>
       <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
+      <c r="H62" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="I62" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="J62" s="4">
+        <v>200</v>
+      </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="N62" s="2">
         <f t="shared" si="1"/>
-        <v>-1.1000000000000001</v>
+        <v>8.5666666666666664</v>
       </c>
       <c r="O62" s="1"/>
-      <c r="P62" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
+      <c r="P62" s="4">
+        <v>-6</v>
+      </c>
+      <c r="Q62" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="R62" s="8">
+        <v>-12</v>
+      </c>
+      <c r="S62" s="8">
+        <v>-11</v>
+      </c>
       <c r="T62" s="4"/>
-      <c r="U62" s="4"/>
-      <c r="V62" s="4"/>
-      <c r="W62" s="4"/>
+      <c r="U62" s="4">
+        <v>-0.15</v>
+      </c>
+      <c r="V62" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="W62" s="4">
+        <v>140</v>
+      </c>
       <c r="X62" s="4"/>
       <c r="Y62" s="4"/>
       <c r="Z62" s="4">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="AA62" s="2">
         <f t="shared" si="2"/>
-        <v>-0.6</v>
+        <v>10.516666666666667</v>
       </c>
       <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
+      <c r="AC62" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="AD62" s="1">
+        <f>AC62*0.015</f>
+        <v>0.20549999999999999</v>
+      </c>
       <c r="AE62" s="1"/>
       <c r="AF62" s="1"/>
       <c r="AG62" s="1"/>
@@ -5683,10 +5705,18 @@
       <c r="AI62" s="1"/>
     </row>
     <row r="63" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
+      <c r="A63" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0.03</v>
+      </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -5695,14 +5725,20 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
+      <c r="M63" s="4">
+        <v>200</v>
+      </c>
       <c r="N63" s="2">
         <f t="shared" si="1"/>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="O63" s="1"/>
+      <c r="P63" s="8">
         <v>0</v>
       </c>
-      <c r="O63" s="1"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
+      <c r="Q63" s="4">
+        <v>0.03</v>
+      </c>
       <c r="R63" s="4"/>
       <c r="S63" s="4"/>
       <c r="T63" s="4"/>
@@ -5711,10 +5747,12 @@
       <c r="W63" s="4"/>
       <c r="X63" s="4"/>
       <c r="Y63" s="4"/>
-      <c r="Z63" s="4"/>
+      <c r="Z63" s="4">
+        <v>200</v>
+      </c>
       <c r="AA63" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.6</v>
       </c>
       <c r="AB63" s="1"/>
       <c r="AC63" s="1"/>
@@ -5726,72 +5764,38 @@
       <c r="AI63" s="1"/>
     </row>
     <row r="64" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C64" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D64" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="F64" s="1">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1">
-        <v>40</v>
-      </c>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1">
-        <v>500</v>
-      </c>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
       <c r="N64" s="2">
         <f t="shared" si="1"/>
-        <v>-2.9666666666666668</v>
+        <v>0</v>
       </c>
       <c r="O64" s="1"/>
-      <c r="P64" s="3">
-        <v>-1</v>
-      </c>
-      <c r="Q64" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="R64" s="1">
-        <v>0</v>
-      </c>
-      <c r="S64" s="1">
-        <v>0</v>
-      </c>
-      <c r="T64" s="1"/>
-      <c r="U64" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="V64" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="W64" s="3">
-        <v>20</v>
-      </c>
-      <c r="X64" s="1"/>
-      <c r="Y64" s="1"/>
-      <c r="Z64" s="1">
-        <v>500</v>
-      </c>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="4"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
+      <c r="Z64" s="4"/>
       <c r="AA64" s="2">
         <f t="shared" si="2"/>
-        <v>-2.2833333333333332</v>
+        <v>0</v>
       </c>
       <c r="AB64" s="1"/>
       <c r="AC64" s="1"/>
@@ -5804,73 +5808,71 @@
     </row>
     <row r="65" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C65" s="1">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="D65" s="1">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E65" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="I65" s="1">
-        <v>0.05</v>
-      </c>
+        <v>0.06</v>
+      </c>
+      <c r="I65" s="1"/>
       <c r="J65" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="N65" s="2">
         <f t="shared" si="1"/>
-        <v>-1.4999999999999998</v>
+        <v>-2.9666666666666668</v>
       </c>
       <c r="O65" s="1"/>
       <c r="P65" s="3">
-        <v>-2</v>
-      </c>
-      <c r="Q65" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="R65" s="3">
+        <v>-1</v>
+      </c>
+      <c r="Q65" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="R65" s="1">
         <v>0</v>
       </c>
-      <c r="S65" s="3">
-        <v>-1</v>
+      <c r="S65" s="1">
+        <v>0</v>
       </c>
       <c r="T65" s="1"/>
       <c r="U65" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="V65" s="3">
-        <v>0.02</v>
+        <v>0.05</v>
+      </c>
+      <c r="V65" s="8">
+        <v>0.01</v>
       </c>
       <c r="W65" s="3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="X65" s="1"/>
       <c r="Y65" s="1"/>
       <c r="Z65" s="1">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="AA65" s="2">
         <f t="shared" si="2"/>
-        <v>-3.7666666666666662</v>
+        <v>-2.2833333333333332</v>
       </c>
       <c r="AB65" s="1"/>
       <c r="AC65" s="1"/>
@@ -5883,73 +5885,73 @@
     </row>
     <row r="66" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C66" s="1">
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="D66" s="1">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="E66" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F66" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="I66" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J66" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="N66" s="2">
         <f t="shared" si="1"/>
-        <v>-2.5333333333333332</v>
+        <v>-1.4999999999999998</v>
       </c>
       <c r="O66" s="1"/>
       <c r="P66" s="3">
-        <v>-3</v>
-      </c>
-      <c r="Q66" s="3">
-        <v>0.17</v>
+        <v>-2</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>0.09</v>
       </c>
       <c r="R66" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="S66" s="3">
         <v>-1</v>
       </c>
       <c r="T66" s="1"/>
       <c r="U66" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="V66" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="W66" s="1">
-        <v>80</v>
+        <v>0.02</v>
+      </c>
+      <c r="W66" s="3">
+        <v>40</v>
       </c>
       <c r="X66" s="1"/>
       <c r="Y66" s="1"/>
       <c r="Z66" s="1">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="AA66" s="2">
         <f t="shared" si="2"/>
-        <v>-6.1333333333333337</v>
+        <v>-3.7666666666666662</v>
       </c>
       <c r="AB66" s="1"/>
       <c r="AC66" s="1"/>
@@ -5961,33 +5963,75 @@
       <c r="AI66" s="1"/>
     </row>
     <row r="67" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="A67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="1">
+        <v>-3</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="E67" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F67" s="1">
+        <v>-2</v>
+      </c>
       <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
+      <c r="H67" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J67" s="1">
+        <v>80</v>
+      </c>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="2"/>
+      <c r="M67" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N67" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.5333333333333332</v>
+      </c>
       <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
+      <c r="P67" s="3">
+        <v>-3</v>
+      </c>
+      <c r="Q67" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="R67" s="3">
+        <v>-1</v>
+      </c>
+      <c r="S67" s="3">
+        <v>-1</v>
+      </c>
       <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
+      <c r="U67" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V67" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="W67" s="1">
+        <v>80</v>
+      </c>
       <c r="X67" s="1"/>
       <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="2"/>
+      <c r="Z67" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AA67" s="2">
+        <f t="shared" si="2"/>
+        <v>-6.1333333333333337</v>
+      </c>
       <c r="AB67" s="1"/>
       <c r="AC67" s="1"/>
       <c r="AD67" s="1"/>
@@ -6093,9 +6137,7 @@
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
-      <c r="V70" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="V70" s="1"/>
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
@@ -6132,7 +6174,9 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
-      <c r="V71" s="1"/>
+      <c r="V71" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
@@ -41445,8 +41489,45 @@
       <c r="AH1025" s="1"/>
       <c r="AI1025" s="1"/>
     </row>
+    <row r="1026" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1"/>
+      <c r="C1026" s="1"/>
+      <c r="D1026" s="1"/>
+      <c r="E1026" s="1"/>
+      <c r="F1026" s="1"/>
+      <c r="G1026" s="1"/>
+      <c r="H1026" s="1"/>
+      <c r="I1026" s="1"/>
+      <c r="J1026" s="1"/>
+      <c r="K1026" s="1"/>
+      <c r="L1026" s="1"/>
+      <c r="M1026" s="1"/>
+      <c r="N1026" s="2"/>
+      <c r="O1026" s="1"/>
+      <c r="P1026" s="1"/>
+      <c r="Q1026" s="1"/>
+      <c r="R1026" s="1"/>
+      <c r="S1026" s="1"/>
+      <c r="T1026" s="1"/>
+      <c r="U1026" s="1"/>
+      <c r="V1026" s="1"/>
+      <c r="W1026" s="1"/>
+      <c r="X1026" s="1"/>
+      <c r="Y1026" s="1"/>
+      <c r="Z1026" s="1"/>
+      <c r="AA1026" s="2"/>
+      <c r="AB1026" s="1"/>
+      <c r="AC1026" s="1"/>
+      <c r="AD1026" s="1"/>
+      <c r="AE1026" s="1"/>
+      <c r="AF1026" s="1"/>
+      <c r="AG1026" s="1"/>
+      <c r="AH1026" s="1"/>
+      <c r="AI1026" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="U3:U63 P3:T66 V3:AA66">
+  <conditionalFormatting sqref="U41:U64 P41:T67 P3:AA40 V41:AA67">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>P3&lt;&gt;C3</formula>
     </cfRule>

</xml_diff>